<commit_message>
Updated few config changes for demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/simple.xlsx
+++ b/src/test/resources/testData/simple.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="qaTestSheetName" sheetId="18" r:id="rId1"/>
     <sheet name="uatTestSheetName" sheetId="17" r:id="rId2"/>
     <sheet name="stageTestSheetName" sheetId="16" r:id="rId3"/>
-    <sheet name="prodTestSheetName" sheetId="19" r:id="rId4"/>
-    <sheet name="xxprodTestSheetName" sheetId="8" r:id="rId5"/>
+    <sheet name="xprodTestSheetName" sheetId="19" r:id="rId4"/>
+    <sheet name="prodTestSheetName" sheetId="8" r:id="rId5"/>
     <sheet name="testLogo" sheetId="15" r:id="rId6"/>
     <sheet name="testSocialShareLinks" sheetId="9" r:id="rId7"/>
   </sheets>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="21">
   <si>
     <t>Runmode</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Automation Testing - Home | Facebook</t>
+  </si>
+  <si>
+    <t>Home Centre India - Home</t>
   </si>
 </sst>
 </file>
@@ -793,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>